<commit_message>
add M in modern sulfur cycle preset profile.dat
</commit_message>
<xml_diff>
--- a/tests/modern_sulfur_cycle/profile.xlsx
+++ b/tests/modern_sulfur_cycle/profile.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1221e7247ec036c5/学术会议/25_10_31 PATMO workshop/Modern sulfur cycle/input files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1221e7247ec036c5/学术会议/25_10_31 PATMO workshop/modern sulfur cycle/input files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="86" documentId="8_{6B81276A-83FB-A843-A3BB-2D87888D32D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7F86F8B-9DAB-8D4C-B3AD-BBEC0B598DEC}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{6B81276A-83FB-A843-A3BB-2D87888D32D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A3CC21A-62C0-49A7-91A5-D5617F5D3F34}"/>
   <bookViews>
-    <workbookView xWindow="17780" yWindow="760" windowWidth="16780" windowHeight="21580" xr2:uid="{D7BD78CA-9E1A-A84E-ABC8-B9A18946ED57}"/>
+    <workbookView xWindow="15735" yWindow="495" windowWidth="22305" windowHeight="20130" xr2:uid="{D7BD78CA-9E1A-A84E-ABC8-B9A18946ED57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -176,12 +176,16 @@
   <si>
     <t>CH4O3S</t>
   </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -229,7 +233,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -244,8 +248,12 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -561,15 +569,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7F68D6-EB94-CE47-9BFF-C3E1342F35B3}">
-  <dimension ref="A1:AI61"/>
+  <dimension ref="A1:AJ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AJ6" sqref="AJ6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -675,8 +683,11 @@
       <c r="AI1" t="s">
         <v>34</v>
       </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -782,8 +793,12 @@
       <c r="AI2" s="1">
         <v>0</v>
       </c>
+      <c r="AJ2" s="1">
+        <f>SUM(F2:AI2)</f>
+        <v>2.3458461978977812E+19</v>
+      </c>
     </row>
-    <row r="3" spans="1:35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -889,8 +904,12 @@
       <c r="AI3" s="1">
         <v>0</v>
       </c>
+      <c r="AJ3" s="1">
+        <f t="shared" ref="AJ3:AJ61" si="0">SUM(F3:AI3)</f>
+        <v>2.0506101918465253E+19</v>
+      </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -996,8 +1015,12 @@
       <c r="AI4" s="1">
         <v>0</v>
       </c>
+      <c r="AJ4" s="1">
+        <f t="shared" si="0"/>
+        <v>1.7915481875072918E+19</v>
+      </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1103,8 +1126,12 @@
       <c r="AI5" s="1">
         <v>0</v>
       </c>
+      <c r="AJ5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5580221866735878E+19</v>
+      </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1210,8 +1237,12 @@
       <c r="AI6" s="1">
         <v>0</v>
       </c>
+      <c r="AJ6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.360684186659686E+19</v>
+      </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1317,8 +1348,12 @@
       <c r="AI7" s="1">
         <v>0</v>
       </c>
+      <c r="AJ7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1820021894510858E+19</v>
+      </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1424,8 +1459,12 @@
       <c r="AI8" s="1">
         <v>0</v>
       </c>
+      <c r="AJ8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0266181988472824E+19</v>
+      </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1531,8 +1570,12 @@
       <c r="AI9" s="1">
         <v>0</v>
       </c>
+      <c r="AJ9" s="1">
+        <f t="shared" si="0"/>
+        <v>8.8936921174446828E+18</v>
+      </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1638,8 +1681,12 @@
       <c r="AI10" s="1">
         <v>0</v>
       </c>
+      <c r="AJ10" s="1">
+        <f t="shared" si="0"/>
+        <v>7.7026204104409477E+18</v>
+      </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1745,8 +1792,12 @@
       <c r="AI11" s="1">
         <v>0</v>
       </c>
+      <c r="AJ11" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6520417004552796E+18</v>
+      </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1852,8 +1903,12 @@
       <c r="AI12" s="1">
         <v>0</v>
       </c>
+      <c r="AJ12" s="1">
+        <f t="shared" si="0"/>
+        <v>5.7916393605054136E+18</v>
+      </c>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1959,8 +2014,12 @@
       <c r="AI13" s="1">
         <v>0</v>
       </c>
+      <c r="AJ13" s="1">
+        <f t="shared" si="0"/>
+        <v>5.0303641106547282E+18</v>
+      </c>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2066,8 +2125,12 @@
       <c r="AI14" s="1">
         <v>0</v>
       </c>
+      <c r="AJ14" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3651407209014164E+18</v>
+      </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2173,8 +2236,12 @@
       <c r="AI15" s="1">
         <v>0</v>
       </c>
+      <c r="AJ15" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7889684911333893E+18</v>
+      </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2280,8 +2347,12 @@
       <c r="AI16" s="1">
         <v>0</v>
       </c>
+      <c r="AJ16" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2898204543859988E+18</v>
+      </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2387,8 +2458,12 @@
       <c r="AI17" s="1">
         <v>0</v>
       </c>
+      <c r="AJ17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8627018896988698E+18</v>
+      </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2494,8 +2569,12 @@
       <c r="AI18" s="1">
         <v>0</v>
       </c>
+      <c r="AJ18" s="1">
+        <f t="shared" si="0"/>
+        <v>2.496599831933525E+18</v>
+      </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2601,8 +2680,12 @@
       <c r="AI19" s="1">
         <v>0</v>
       </c>
+      <c r="AJ19" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1705150580853883E+18</v>
+      </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2708,8 +2791,12 @@
       <c r="AI20" s="1">
         <v>0</v>
       </c>
+      <c r="AJ20" s="1">
+        <f t="shared" si="0"/>
+        <v>1.891443327259073E+18</v>
+      </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2815,8 +2902,12 @@
       <c r="AI21" s="1">
         <v>0</v>
       </c>
+      <c r="AJ21" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6503816621814341E+18</v>
+      </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2922,8 +3013,12 @@
       <c r="AI22" s="1">
         <v>0</v>
       </c>
+      <c r="AJ22" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4383349377057398E+18</v>
+      </c>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3029,8 +3124,12 @@
       <c r="AI23" s="1">
         <v>0</v>
       </c>
+      <c r="AJ23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2512941222786401E+18</v>
+      </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3136,8 +3235,12 @@
       <c r="AI24" s="1">
         <v>0</v>
       </c>
+      <c r="AJ24" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0952604414841201E+18</v>
+      </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3243,8 +3346,12 @@
       <c r="AI25" s="1">
         <v>0</v>
       </c>
+      <c r="AJ25" s="1">
+        <f t="shared" si="0"/>
+        <v>9.562304645460201E+17</v>
+      </c>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3350,8 +3457,12 @@
       <c r="AI26" s="1">
         <v>0</v>
       </c>
+      <c r="AJ26" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3520553765064998E+17</v>
+      </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3457,8 +3568,12 @@
       <c r="AI27" s="1">
         <v>0</v>
       </c>
+      <c r="AJ27" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2918256259629005E+17</v>
+      </c>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3564,8 +3679,12 @@
       <c r="AI28" s="1">
         <v>0</v>
       </c>
+      <c r="AJ28" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3696006820036992E+17</v>
+      </c>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3671,8 +3790,12 @@
       <c r="AI29" s="1">
         <v>0</v>
       </c>
+      <c r="AJ29" s="1">
+        <f t="shared" si="0"/>
+        <v>5.5654091503363994E+17</v>
+      </c>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3778,8 +3901,12 @@
       <c r="AI30" s="1">
         <v>0</v>
       </c>
+      <c r="AJ30" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8662401241907008E+17</v>
+      </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3885,8 +4012,12 @@
       <c r="AI31" s="1">
         <v>0</v>
       </c>
+      <c r="AJ31" s="1">
+        <f t="shared" si="0"/>
+        <v>4.2500945015676998E+17</v>
+      </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3992,8 +4123,12 @@
       <c r="AI32" s="1">
         <v>0</v>
       </c>
+      <c r="AJ32" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7269841843614003E+17</v>
+      </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4099,8 +4234,12 @@
       <c r="AI33" s="1">
         <v>0</v>
       </c>
+      <c r="AJ33" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2708826699749997E+17</v>
+      </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4206,8 +4345,12 @@
       <c r="AI34" s="1">
         <v>0</v>
       </c>
+      <c r="AJ34" s="1">
+        <f t="shared" si="0"/>
+        <v>2.870789257714E+17</v>
+      </c>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4313,8 +4456,12 @@
       <c r="AI35" s="1">
         <v>0</v>
       </c>
+      <c r="AJ35" s="1">
+        <f t="shared" si="0"/>
+        <v>2.517706647337E+17</v>
+      </c>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4420,8 +4567,12 @@
       <c r="AI36" s="1">
         <v>0</v>
       </c>
+      <c r="AJ36" s="1">
+        <f t="shared" si="0"/>
+        <v>2.208634637075E+17</v>
+      </c>
     </row>
-    <row r="37" spans="1:35">
+    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4527,8 +4678,12 @@
       <c r="AI37" s="1">
         <v>0</v>
       </c>
+      <c r="AJ37" s="1">
+        <f t="shared" si="0"/>
+        <v>1.949570227853E+17</v>
+      </c>
     </row>
-    <row r="38" spans="1:35">
+    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4634,8 +4789,12 @@
       <c r="AI38" s="1">
         <v>0</v>
       </c>
+      <c r="AJ38" s="1">
+        <f t="shared" si="0"/>
+        <v>1.713522522366E+17</v>
+      </c>
     </row>
-    <row r="39" spans="1:35">
+    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4741,8 +4900,12 @@
       <c r="AI39" s="1">
         <v>0</v>
       </c>
+      <c r="AJ39" s="1">
+        <f t="shared" si="0"/>
+        <v>1.520479918298E+17</v>
+      </c>
     </row>
-    <row r="40" spans="1:35">
+    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4848,8 +5011,12 @@
       <c r="AI40" s="1">
         <v>0</v>
       </c>
+      <c r="AJ40" s="1">
+        <f t="shared" si="0"/>
+        <v>1.33844261567E+17</v>
+      </c>
     </row>
-    <row r="41" spans="1:35">
+    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4955,8 +5122,12 @@
       <c r="AI41" s="1">
         <v>0</v>
       </c>
+      <c r="AJ41" s="1">
+        <f t="shared" si="0"/>
+        <v>1.18240026433E+17</v>
+      </c>
     </row>
-    <row r="42" spans="1:35">
+    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5062,8 +5233,12 @@
       <c r="AI42" s="1">
         <v>0</v>
       </c>
+      <c r="AJ42" s="1">
+        <f t="shared" si="0"/>
+        <v>1.045368914177E+17</v>
+      </c>
     </row>
-    <row r="43" spans="1:35">
+    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5169,8 +5344,12 @@
       <c r="AI43" s="1">
         <v>0</v>
       </c>
+      <c r="AJ43" s="1">
+        <f t="shared" si="0"/>
+        <v>9.25341416437E+16</v>
+      </c>
     </row>
-    <row r="44" spans="1:35">
+    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5276,8 +5455,12 @@
       <c r="AI44" s="1">
         <v>0</v>
       </c>
+      <c r="AJ44" s="1">
+        <f t="shared" si="0"/>
+        <v>8.20316630135E+16</v>
+      </c>
     </row>
-    <row r="45" spans="1:35">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5383,8 +5566,12 @@
       <c r="AI45" s="1">
         <v>0</v>
       </c>
+      <c r="AJ45" s="1">
+        <f t="shared" si="0"/>
+        <v>7.28288865226E+16</v>
+      </c>
     </row>
-    <row r="46" spans="1:35">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5490,8 +5677,12 @@
       <c r="AI46" s="1">
         <v>0</v>
       </c>
+      <c r="AJ46" s="1">
+        <f t="shared" si="0"/>
+        <v>6.47269522163E+16</v>
+      </c>
     </row>
-    <row r="47" spans="1:35">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5597,8 +5788,12 @@
       <c r="AI47" s="1">
         <v>0</v>
       </c>
+      <c r="AJ47" s="1">
+        <f t="shared" si="0"/>
+        <v>5.74251690483E+16</v>
+      </c>
     </row>
-    <row r="48" spans="1:35">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5704,8 +5899,12 @@
       <c r="AI48" s="1">
         <v>0</v>
       </c>
+      <c r="AJ48" s="1">
+        <f t="shared" si="0"/>
+        <v>5.072251598238E+16</v>
+      </c>
     </row>
-    <row r="49" spans="1:35">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5811,8 +6010,12 @@
       <c r="AI49" s="1">
         <v>0</v>
       </c>
+      <c r="AJ49" s="1">
+        <f t="shared" si="0"/>
+        <v>4.472018993666E+16</v>
+      </c>
     </row>
-    <row r="50" spans="1:35">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5918,8 +6121,12 @@
       <c r="AI50" s="1">
         <v>0</v>
       </c>
+      <c r="AJ50" s="1">
+        <f t="shared" si="0"/>
+        <v>3.951857390461E+16</v>
+      </c>
     </row>
-    <row r="51" spans="1:35">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6025,8 +6232,12 @@
       <c r="AI51" s="1">
         <v>0</v>
       </c>
+      <c r="AJ51" s="1">
+        <f t="shared" si="0"/>
+        <v>3.461628182444E+16</v>
+      </c>
     </row>
-    <row r="52" spans="1:35">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6132,8 +6343,12 @@
       <c r="AI52" s="1">
         <v>0</v>
       </c>
+      <c r="AJ52" s="1">
+        <f t="shared" si="0"/>
+        <v>3.029431548183E+16</v>
+      </c>
     </row>
-    <row r="53" spans="1:35">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6239,8 +6454,12 @@
       <c r="AI53" s="1">
         <v>0</v>
       </c>
+      <c r="AJ53" s="1">
+        <f t="shared" si="0"/>
+        <v>2.608167338304E+16</v>
+      </c>
     </row>
-    <row r="54" spans="1:35">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -6346,8 +6565,12 @@
       <c r="AI54" s="1">
         <v>0</v>
       </c>
+      <c r="AJ54" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2499754795633E+16</v>
+      </c>
     </row>
-    <row r="55" spans="1:35">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -6453,8 +6676,12 @@
       <c r="AI55" s="1">
         <v>0</v>
       </c>
+      <c r="AJ55" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9318150493472E+16</v>
+      </c>
     </row>
-    <row r="56" spans="1:35">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6560,8 +6787,12 @@
       <c r="AI56" s="1">
         <v>0</v>
       </c>
+      <c r="AJ56" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6616615191464E+16</v>
+      </c>
     </row>
-    <row r="57" spans="1:35">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6667,8 +6898,12 @@
       <c r="AI57" s="1">
         <v>0</v>
       </c>
+      <c r="AJ57" s="1">
+        <f t="shared" si="0"/>
+        <v>1.4255497796014E+16</v>
+      </c>
     </row>
-    <row r="58" spans="1:35">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6774,8 +7009,12 @@
       <c r="AI58" s="1">
         <v>0</v>
       </c>
+      <c r="AJ58" s="1">
+        <f t="shared" si="0"/>
+        <v>1.2304429994239E+16</v>
+      </c>
     </row>
-    <row r="59" spans="1:35">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6881,8 +7120,12 @@
       <c r="AI59" s="1">
         <v>0</v>
       </c>
+      <c r="AJ59" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0583657799677E+16</v>
+      </c>
     </row>
-    <row r="60" spans="1:35">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -6988,8 +7231,12 @@
       <c r="AI60" s="1">
         <v>0</v>
       </c>
+      <c r="AJ60" s="1">
+        <f t="shared" si="0"/>
+        <v>9103021704929600</v>
+      </c>
     </row>
-    <row r="61" spans="1:35">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -7094,6 +7341,10 @@
       </c>
       <c r="AI61" s="1">
         <v>0</v>
+      </c>
+      <c r="AJ61" s="1">
+        <f t="shared" si="0"/>
+        <v>7712271690540800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix issues for modern sulfur cycle preset
</commit_message>
<xml_diff>
--- a/tests/modern_sulfur_cycle/profile.xlsx
+++ b/tests/modern_sulfur_cycle/profile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1221e7247ec036c5/学术会议/25_10_31 PATMO workshop/modern sulfur cycle/input files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{6B81276A-83FB-A843-A3BB-2D87888D32D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A3CC21A-62C0-49A7-91A5-D5617F5D3F34}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{6B81276A-83FB-A843-A3BB-2D87888D32D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{425D96BA-B7AB-4C39-96F8-A5598B36CC79}"/>
   <bookViews>
-    <workbookView xWindow="15735" yWindow="495" windowWidth="22305" windowHeight="20130" xr2:uid="{D7BD78CA-9E1A-A84E-ABC8-B9A18946ED57}"/>
+    <workbookView xWindow="11610" yWindow="750" windowWidth="22305" windowHeight="20130" xr2:uid="{D7BD78CA-9E1A-A84E-ABC8-B9A18946ED57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -91,10 +91,6 @@
   </si>
   <si>
     <t>H2O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NO2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -569,15 +565,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA7F68D6-EB94-CE47-9BFF-C3E1342F35B3}">
-  <dimension ref="A1:AJ61"/>
+  <dimension ref="A1:AI61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AJ6" sqref="AJ6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,11 +679,8 @@
       <c r="AI1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
-      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -731,7 +724,7 @@
         <v>1.5E+17</v>
       </c>
       <c r="O2" s="1">
-        <v>1370000000</v>
+        <v>0</v>
       </c>
       <c r="P2" s="1">
         <v>0</v>
@@ -791,14 +784,11 @@
         <v>0</v>
       </c>
       <c r="AI2" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="1">
-        <f>SUM(F2:AI2)</f>
-        <v>2.3458461978977812E+19</v>
+        <f>SUM(F2:AH2)</f>
+        <v>2.3458461977607811E+19</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -842,7 +832,7 @@
         <v>8.95E+16</v>
       </c>
       <c r="O3" s="1">
-        <v>1000000000</v>
+        <v>0</v>
       </c>
       <c r="P3" s="1">
         <v>0</v>
@@ -902,14 +892,11 @@
         <v>0</v>
       </c>
       <c r="AI3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="1">
-        <f t="shared" ref="AJ3:AJ61" si="0">SUM(F3:AI3)</f>
-        <v>2.0506101918465253E+19</v>
+        <f t="shared" ref="AI3:AI61" si="0">SUM(F3:AH3)</f>
+        <v>2.0506101917465252E+19</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -953,7 +940,7 @@
         <v>4.97E+16</v>
       </c>
       <c r="O4" s="1">
-        <v>696000000</v>
+        <v>0</v>
       </c>
       <c r="P4" s="1">
         <v>0</v>
@@ -1013,14 +1000,11 @@
         <v>0</v>
       </c>
       <c r="AI4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="1">
         <f t="shared" si="0"/>
-        <v>1.7915481875072918E+19</v>
+        <v>1.7915481874376917E+19</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1064,7 +1048,7 @@
         <v>2.52E+16</v>
       </c>
       <c r="O5" s="1">
-        <v>508000000</v>
+        <v>0</v>
       </c>
       <c r="P5" s="1">
         <v>0</v>
@@ -1124,14 +1108,11 @@
         <v>0</v>
       </c>
       <c r="AI5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="1">
         <f t="shared" si="0"/>
-        <v>1.5580221866735878E+19</v>
+        <v>1.5580221866227878E+19</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1175,7 +1156,7 @@
         <v>1.25E+16</v>
       </c>
       <c r="O6" s="1">
-        <v>412000000</v>
+        <v>0</v>
       </c>
       <c r="P6" s="1">
         <v>0</v>
@@ -1235,14 +1216,11 @@
         <v>0</v>
       </c>
       <c r="AI6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="1">
         <f t="shared" si="0"/>
-        <v>1.360684186659686E+19</v>
+        <v>1.360684186618486E+19</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1286,7 +1264,7 @@
         <v>6310000000000000</v>
       </c>
       <c r="O7" s="1">
-        <v>381000000</v>
+        <v>0</v>
       </c>
       <c r="P7" s="1">
         <v>0</v>
@@ -1346,14 +1324,11 @@
         <v>0</v>
       </c>
       <c r="AI7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="1">
         <f t="shared" si="0"/>
-        <v>1.1820021894510858E+19</v>
+        <v>1.1820021894129859E+19</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1397,7 +1372,7 @@
         <v>3020000000000000</v>
       </c>
       <c r="O8" s="1">
-        <v>371000000</v>
+        <v>0</v>
       </c>
       <c r="P8" s="1">
         <v>0</v>
@@ -1457,14 +1432,11 @@
         <v>0</v>
       </c>
       <c r="AI8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="1">
         <f t="shared" si="0"/>
-        <v>1.0266181988472824E+19</v>
+        <v>1.0266181988101825E+19</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1508,7 +1480,7 @@
         <v>1040000000000000</v>
       </c>
       <c r="O9" s="1">
-        <v>371000000</v>
+        <v>0</v>
       </c>
       <c r="P9" s="1">
         <v>0</v>
@@ -1568,14 +1540,11 @@
         <v>0</v>
       </c>
       <c r="AI9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="1">
         <f t="shared" si="0"/>
-        <v>8.8936921174446828E+18</v>
+        <v>8.8936921170736824E+18</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1619,7 +1588,7 @@
         <v>398000000000000</v>
       </c>
       <c r="O10" s="1">
-        <v>381000000</v>
+        <v>0</v>
       </c>
       <c r="P10" s="1">
         <v>0</v>
@@ -1679,14 +1648,11 @@
         <v>0</v>
       </c>
       <c r="AI10" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="1">
         <f t="shared" si="0"/>
-        <v>7.7026204104409477E+18</v>
+        <v>7.702620410059948E+18</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1730,7 +1696,7 @@
         <v>189000000000000</v>
       </c>
       <c r="O11" s="1">
-        <v>402000000</v>
+        <v>0</v>
       </c>
       <c r="P11" s="1">
         <v>0</v>
@@ -1790,14 +1756,11 @@
         <v>0</v>
       </c>
       <c r="AI11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="1">
         <f t="shared" si="0"/>
-        <v>6.6520417004552796E+18</v>
+        <v>6.6520417000532797E+18</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1841,7 +1804,7 @@
         <v>96400000000000</v>
       </c>
       <c r="O12" s="1">
-        <v>458000000</v>
+        <v>0</v>
       </c>
       <c r="P12" s="1">
         <v>0</v>
@@ -1901,14 +1864,11 @@
         <v>0</v>
       </c>
       <c r="AI12" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ12" s="1">
         <f t="shared" si="0"/>
-        <v>5.7916393605054136E+18</v>
+        <v>5.7916393600474132E+18</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1952,7 +1912,7 @@
         <v>51000000000000</v>
       </c>
       <c r="O13" s="1">
-        <v>610000000</v>
+        <v>0</v>
       </c>
       <c r="P13" s="1">
         <v>0</v>
@@ -2012,14 +1972,11 @@
         <v>0</v>
       </c>
       <c r="AI13" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="1">
         <f t="shared" si="0"/>
-        <v>5.0303641106547282E+18</v>
+        <v>5.0303641100447283E+18</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2063,7 +2020,7 @@
         <v>27500000000000</v>
       </c>
       <c r="O14" s="1">
-        <v>858000000</v>
+        <v>0</v>
       </c>
       <c r="P14" s="1">
         <v>0</v>
@@ -2123,14 +2080,11 @@
         <v>0</v>
       </c>
       <c r="AI14" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ14" s="1">
         <f t="shared" si="0"/>
-        <v>4.3651407209014164E+18</v>
+        <v>4.3651407200434166E+18</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2174,7 +2128,7 @@
         <v>24100000000000</v>
       </c>
       <c r="O15" s="1">
-        <v>1090000000</v>
+        <v>0</v>
       </c>
       <c r="P15" s="1">
         <v>0</v>
@@ -2234,14 +2188,11 @@
         <v>0</v>
       </c>
       <c r="AI15" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ15" s="1">
         <f t="shared" si="0"/>
-        <v>3.7889684911333893E+18</v>
+        <v>3.7889684900433894E+18</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2285,7 +2236,7 @@
         <v>20900000000000</v>
       </c>
       <c r="O16" s="1">
-        <v>1340000000</v>
+        <v>0</v>
       </c>
       <c r="P16" s="1">
         <v>0</v>
@@ -2345,14 +2296,11 @@
         <v>0</v>
       </c>
       <c r="AI16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ16" s="1">
         <f t="shared" si="0"/>
-        <v>3.2898204543859988E+18</v>
+        <v>3.2898204530459991E+18</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2396,7 +2344,7 @@
         <v>18200000000000</v>
       </c>
       <c r="O17" s="1">
-        <v>1650000000</v>
+        <v>0</v>
       </c>
       <c r="P17" s="1">
         <v>0</v>
@@ -2456,14 +2404,11 @@
         <v>0</v>
       </c>
       <c r="AI17" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ17" s="1">
         <f t="shared" si="0"/>
-        <v>2.8627018896988698E+18</v>
+        <v>2.8627018880488699E+18</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2507,7 +2452,7 @@
         <v>15800000000000</v>
       </c>
       <c r="O18" s="1">
-        <v>1880000000</v>
+        <v>0</v>
       </c>
       <c r="P18" s="1">
         <v>0</v>
@@ -2567,14 +2512,11 @@
         <v>0</v>
       </c>
       <c r="AI18" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ18" s="1">
         <f t="shared" si="0"/>
-        <v>2.496599831933525E+18</v>
+        <v>2.496599830053525E+18</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2618,7 +2560,7 @@
         <v>14700000000000</v>
       </c>
       <c r="O19" s="1">
-        <v>2030000000</v>
+        <v>0</v>
       </c>
       <c r="P19" s="1">
         <v>0</v>
@@ -2678,14 +2620,11 @@
         <v>0</v>
       </c>
       <c r="AI19" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ19" s="1">
         <f t="shared" si="0"/>
-        <v>2.1705150580853883E+18</v>
+        <v>2.1705150560553882E+18</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2729,7 +2668,7 @@
         <v>14700000000000</v>
       </c>
       <c r="O20" s="1">
-        <v>2200000000</v>
+        <v>0</v>
       </c>
       <c r="P20" s="1">
         <v>0</v>
@@ -2789,14 +2728,11 @@
         <v>0</v>
       </c>
       <c r="AI20" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ20" s="1">
         <f t="shared" si="0"/>
-        <v>1.891443327259073E+18</v>
+        <v>1.891443325059073E+18</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2840,7 +2776,7 @@
         <v>14900000000000</v>
       </c>
       <c r="O21" s="1">
-        <v>2320000000</v>
+        <v>0</v>
       </c>
       <c r="P21" s="1">
         <v>0</v>
@@ -2900,14 +2836,11 @@
         <v>0</v>
       </c>
       <c r="AI21" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ21" s="1">
         <f t="shared" si="0"/>
-        <v>1.6503816621814341E+18</v>
+        <v>1.6503816598614341E+18</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2951,7 +2884,7 @@
         <v>16100000000000</v>
       </c>
       <c r="O22" s="1">
-        <v>2440000000</v>
+        <v>0</v>
       </c>
       <c r="P22" s="1">
         <v>0</v>
@@ -3011,14 +2944,11 @@
         <v>0</v>
       </c>
       <c r="AI22" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ22" s="1">
         <f t="shared" si="0"/>
-        <v>1.4383349377057398E+18</v>
+        <v>1.4383349352657398E+18</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3062,7 +2992,7 @@
         <v>17200000000000</v>
       </c>
       <c r="O23" s="1">
-        <v>2510000000</v>
+        <v>0</v>
       </c>
       <c r="P23" s="1">
         <v>0</v>
@@ -3122,14 +3052,11 @@
         <v>0</v>
       </c>
       <c r="AI23" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ23" s="1">
         <f t="shared" si="0"/>
-        <v>1.2512941222786401E+18</v>
+        <v>1.25129411976864E+18</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3173,7 +3100,7 @@
         <v>18600000000000</v>
       </c>
       <c r="O24" s="1">
-        <v>2510000000</v>
+        <v>0</v>
       </c>
       <c r="P24" s="1">
         <v>0</v>
@@ -3233,14 +3160,11 @@
         <v>0</v>
       </c>
       <c r="AI24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="1">
         <f t="shared" si="0"/>
-        <v>1.0952604414841201E+18</v>
+        <v>1.0952604389741201E+18</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3284,7 +3208,7 @@
         <v>19800000000000</v>
       </c>
       <c r="O25" s="1">
-        <v>2570000000</v>
+        <v>0</v>
       </c>
       <c r="P25" s="1">
         <v>0</v>
@@ -3344,14 +3268,11 @@
         <v>0</v>
       </c>
       <c r="AI25" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ25" s="1">
         <f t="shared" si="0"/>
-        <v>9.562304645460201E+17</v>
+        <v>9.562304619760201E+17</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3395,7 +3316,7 @@
         <v>21100000000000</v>
       </c>
       <c r="O26" s="1">
-        <v>2570000000</v>
+        <v>0</v>
       </c>
       <c r="P26" s="1">
         <v>0</v>
@@ -3455,14 +3376,11 @@
         <v>0</v>
       </c>
       <c r="AI26" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ26" s="1">
         <f t="shared" si="0"/>
-        <v>8.3520553765064998E+17</v>
+        <v>8.3520553508064998E+17</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3506,7 +3424,7 @@
         <v>21400000000000</v>
       </c>
       <c r="O27" s="1">
-        <v>2510000000</v>
+        <v>0</v>
       </c>
       <c r="P27" s="1">
         <v>0</v>
@@ -3566,14 +3484,11 @@
         <v>0</v>
       </c>
       <c r="AI27" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ27" s="1">
         <f t="shared" si="0"/>
-        <v>7.2918256259629005E+17</v>
+        <v>7.2918256008629005E+17</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3617,7 +3532,7 @@
         <v>19300000000000</v>
       </c>
       <c r="O28" s="1">
-        <v>2510000000</v>
+        <v>0</v>
       </c>
       <c r="P28" s="1">
         <v>0</v>
@@ -3677,14 +3592,11 @@
         <v>0</v>
       </c>
       <c r="AI28" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ28" s="1">
         <f t="shared" si="0"/>
-        <v>6.3696006820036992E+17</v>
+        <v>6.3696006569036992E+17</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3728,7 +3640,7 @@
         <v>17500000000000</v>
       </c>
       <c r="O29" s="1">
-        <v>2440000000</v>
+        <v>0</v>
       </c>
       <c r="P29" s="1">
         <v>0</v>
@@ -3788,14 +3700,11 @@
         <v>0</v>
       </c>
       <c r="AI29" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ29" s="1">
         <f t="shared" si="0"/>
-        <v>5.5654091503363994E+17</v>
+        <v>5.5654091259363994E+17</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3839,7 +3748,7 @@
         <v>15900000000000</v>
       </c>
       <c r="O30" s="1">
-        <v>2320000000</v>
+        <v>0</v>
       </c>
       <c r="P30" s="1">
         <v>0</v>
@@ -3899,14 +3808,11 @@
         <v>0</v>
       </c>
       <c r="AI30" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ30" s="1">
         <f t="shared" si="0"/>
-        <v>4.8662401241907008E+17</v>
+        <v>4.8662401009907008E+17</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3950,7 +3856,7 @@
         <v>14500000000000</v>
       </c>
       <c r="O31" s="1">
-        <v>2200000000</v>
+        <v>0</v>
       </c>
       <c r="P31" s="1">
         <v>0</v>
@@ -4010,14 +3916,11 @@
         <v>0</v>
       </c>
       <c r="AI31" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ31" s="1">
         <f t="shared" si="0"/>
-        <v>4.2500945015676998E+17</v>
+        <v>4.2500944795676998E+17</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4061,7 +3964,7 @@
         <v>13200000000000</v>
       </c>
       <c r="O32" s="1">
-        <v>2030000000</v>
+        <v>0</v>
       </c>
       <c r="P32" s="1">
         <v>0</v>
@@ -4121,14 +4024,11 @@
         <v>0</v>
       </c>
       <c r="AI32" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ32" s="1">
         <f t="shared" si="0"/>
-        <v>3.7269841843614003E+17</v>
+        <v>3.7269841640614003E+17</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4172,7 +4072,7 @@
         <v>11800000000000</v>
       </c>
       <c r="O33" s="1">
-        <v>1830000000</v>
+        <v>0</v>
       </c>
       <c r="P33" s="1">
         <v>0</v>
@@ -4232,14 +4132,11 @@
         <v>0</v>
       </c>
       <c r="AI33" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ33" s="1">
         <f t="shared" si="0"/>
-        <v>3.2708826699749997E+17</v>
+        <v>3.2708826516749997E+17</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4283,7 +4180,7 @@
         <v>10200000000000</v>
       </c>
       <c r="O34" s="1">
-        <v>1690000000</v>
+        <v>0</v>
       </c>
       <c r="P34" s="1">
         <v>0</v>
@@ -4343,14 +4240,11 @@
         <v>0</v>
       </c>
       <c r="AI34" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ34" s="1">
         <f t="shared" si="0"/>
-        <v>2.870789257714E+17</v>
+        <v>2.870789240814E+17</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4394,7 +4288,7 @@
         <v>8760000000000</v>
       </c>
       <c r="O35" s="1">
-        <v>1410000000</v>
+        <v>0</v>
       </c>
       <c r="P35" s="1">
         <v>0</v>
@@ -4454,14 +4348,11 @@
         <v>0</v>
       </c>
       <c r="AI35" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ35" s="1">
         <f t="shared" si="0"/>
-        <v>2.517706647337E+17</v>
+        <v>2.517706633237E+17</v>
       </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4505,7 +4396,7 @@
         <v>7540000000000</v>
       </c>
       <c r="O36" s="1">
-        <v>1210000000</v>
+        <v>0</v>
       </c>
       <c r="P36" s="1">
         <v>0</v>
@@ -4565,14 +4456,11 @@
         <v>0</v>
       </c>
       <c r="AI36" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ36" s="1">
         <f t="shared" si="0"/>
-        <v>2.208634637075E+17</v>
+        <v>2.208634624975E+17</v>
       </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4616,7 +4504,7 @@
         <v>6470000000000</v>
       </c>
       <c r="O37" s="1">
-        <v>952000000</v>
+        <v>0</v>
       </c>
       <c r="P37" s="1">
         <v>0</v>
@@ -4676,14 +4564,11 @@
         <v>0</v>
       </c>
       <c r="AI37" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ37" s="1">
         <f t="shared" si="0"/>
-        <v>1.949570227853E+17</v>
+        <v>1.949570218333E+17</v>
       </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4727,7 +4612,7 @@
         <v>5540000000000</v>
       </c>
       <c r="O38" s="1">
-        <v>714000000</v>
+        <v>0</v>
       </c>
       <c r="P38" s="1">
         <v>0</v>
@@ -4787,14 +4672,11 @@
         <v>0</v>
       </c>
       <c r="AI38" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ38" s="1">
         <f t="shared" si="0"/>
-        <v>1.713522522366E+17</v>
+        <v>1.713522515226E+17</v>
       </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4838,7 +4720,7 @@
         <v>4760000000000</v>
       </c>
       <c r="O39" s="1">
-        <v>508000000</v>
+        <v>0</v>
       </c>
       <c r="P39" s="1">
         <v>0</v>
@@ -4898,14 +4780,11 @@
         <v>0</v>
       </c>
       <c r="AI39" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ39" s="1">
         <f t="shared" si="0"/>
-        <v>1.520479918298E+17</v>
+        <v>1.520479913218E+17</v>
       </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4949,7 +4828,7 @@
         <v>4090000000000</v>
       </c>
       <c r="O40" s="1">
-        <v>381000000</v>
+        <v>0</v>
       </c>
       <c r="P40" s="1">
         <v>0</v>
@@ -5009,14 +4888,11 @@
         <v>0</v>
       </c>
       <c r="AI40" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ40" s="1">
         <f t="shared" si="0"/>
-        <v>1.33844261567E+17</v>
+        <v>1.33844261186E+17</v>
       </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5060,7 +4936,7 @@
         <v>3500000000000</v>
       </c>
       <c r="O41" s="1">
-        <v>238000000</v>
+        <v>0</v>
       </c>
       <c r="P41" s="1">
         <v>0</v>
@@ -5120,14 +4996,11 @@
         <v>0</v>
       </c>
       <c r="AI41" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ41" s="1">
         <f t="shared" si="0"/>
-        <v>1.18240026433E+17</v>
+        <v>1.18240026195E+17</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5171,7 +5044,7 @@
         <v>2990000000000</v>
       </c>
       <c r="O42" s="1">
-        <v>178000000</v>
+        <v>0</v>
       </c>
       <c r="P42" s="1">
         <v>0</v>
@@ -5231,14 +5104,11 @@
         <v>0</v>
       </c>
       <c r="AI42" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ42" s="1">
         <f t="shared" si="0"/>
-        <v>1.045368914177E+17</v>
+        <v>1.045368912397E+17</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5282,7 +5152,7 @@
         <v>2550000000000</v>
       </c>
       <c r="O43" s="1">
-        <v>109000000</v>
+        <v>0</v>
       </c>
       <c r="P43" s="1">
         <v>0</v>
@@ -5342,14 +5212,11 @@
         <v>0</v>
       </c>
       <c r="AI43" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ43" s="1">
         <f t="shared" si="0"/>
-        <v>9.25341416437E+16</v>
+        <v>9.25341415347E+16</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5393,7 +5260,7 @@
         <v>2170000000000</v>
       </c>
       <c r="O44" s="1">
-        <v>71400000</v>
+        <v>0</v>
       </c>
       <c r="P44" s="1">
         <v>0</v>
@@ -5453,14 +5320,11 @@
         <v>0</v>
       </c>
       <c r="AI44" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ44" s="1">
         <f t="shared" si="0"/>
-        <v>8.20316630135E+16</v>
+        <v>8.20316629421E+16</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5504,7 +5368,7 @@
         <v>1890000000000</v>
       </c>
       <c r="O45" s="1">
-        <v>48200000</v>
+        <v>0</v>
       </c>
       <c r="P45" s="1">
         <v>0</v>
@@ -5564,14 +5428,11 @@
         <v>0</v>
       </c>
       <c r="AI45" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ45" s="1">
         <f t="shared" si="0"/>
-        <v>7.28288865226E+16</v>
+        <v>7.28288864744E+16</v>
       </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5615,7 +5476,7 @@
         <v>1640000000000</v>
       </c>
       <c r="O46" s="1">
-        <v>29300000</v>
+        <v>0</v>
       </c>
       <c r="P46" s="1">
         <v>0</v>
@@ -5675,14 +5536,11 @@
         <v>0</v>
       </c>
       <c r="AI46" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ46" s="1">
         <f t="shared" si="0"/>
-        <v>6.47269522163E+16</v>
+        <v>6.4726952187E+16</v>
       </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5726,7 +5584,7 @@
         <v>1430000000000</v>
       </c>
       <c r="O47" s="1">
-        <v>16900000</v>
+        <v>0</v>
       </c>
       <c r="P47" s="1">
         <v>0</v>
@@ -5786,14 +5644,11 @@
         <v>0</v>
       </c>
       <c r="AI47" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ47" s="1">
         <f t="shared" si="0"/>
-        <v>5.74251690483E+16</v>
+        <v>5.74251690314E+16</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5837,7 +5692,7 @@
         <v>1240000000000</v>
       </c>
       <c r="O48" s="1">
-        <v>9780000</v>
+        <v>0</v>
       </c>
       <c r="P48" s="1">
         <v>0</v>
@@ -5897,14 +5752,11 @@
         <v>0</v>
       </c>
       <c r="AI48" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ48" s="1">
         <f t="shared" si="0"/>
-        <v>5.072251598238E+16</v>
+        <v>5.07225159726E+16</v>
       </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5948,7 +5800,7 @@
         <v>1070000000000</v>
       </c>
       <c r="O49" s="1">
-        <v>6960000</v>
+        <v>0</v>
       </c>
       <c r="P49" s="1">
         <v>0</v>
@@ -6008,14 +5860,11 @@
         <v>0</v>
       </c>
       <c r="AI49" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ49" s="1">
         <f t="shared" si="0"/>
-        <v>4.472018993666E+16</v>
+        <v>4.47201899297E+16</v>
       </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6059,7 +5908,7 @@
         <v>896000000000</v>
       </c>
       <c r="O50" s="1">
-        <v>3910000</v>
+        <v>0</v>
       </c>
       <c r="P50" s="1">
         <v>0</v>
@@ -6119,14 +5968,11 @@
         <v>0</v>
       </c>
       <c r="AI50" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ50" s="1">
         <f t="shared" si="0"/>
-        <v>3.951857390461E+16</v>
+        <v>3.95185739007E+16</v>
       </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6170,7 +6016,7 @@
         <v>741000000000</v>
       </c>
       <c r="O51" s="1">
-        <v>2640000</v>
+        <v>0</v>
       </c>
       <c r="P51" s="1">
         <v>0</v>
@@ -6230,14 +6076,11 @@
         <v>0</v>
       </c>
       <c r="AI51" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ51" s="1">
         <f t="shared" si="0"/>
-        <v>3.461628182444E+16</v>
+        <v>3.46162818218E+16</v>
       </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6281,7 +6124,7 @@
         <v>606000000000</v>
       </c>
       <c r="O52" s="1">
-        <v>1830000</v>
+        <v>0</v>
       </c>
       <c r="P52" s="1">
         <v>0</v>
@@ -6341,14 +6184,11 @@
         <v>0</v>
       </c>
       <c r="AI52" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ52" s="1">
         <f t="shared" si="0"/>
-        <v>3.029431548183E+16</v>
+        <v>3.029431548E+16</v>
       </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -6392,7 +6232,7 @@
         <v>487000000000</v>
       </c>
       <c r="O53" s="1">
-        <v>1140000</v>
+        <v>0</v>
       </c>
       <c r="P53" s="1">
         <v>0</v>
@@ -6452,14 +6292,11 @@
         <v>0</v>
       </c>
       <c r="AI53" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ53" s="1">
         <f t="shared" si="0"/>
-        <v>2.608167338304E+16</v>
+        <v>2.60816733819E+16</v>
       </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -6503,7 +6340,7 @@
         <v>391000000000</v>
       </c>
       <c r="O54" s="1">
-        <v>733000</v>
+        <v>0</v>
       </c>
       <c r="P54" s="1">
         <v>0</v>
@@ -6563,14 +6400,11 @@
         <v>0</v>
       </c>
       <c r="AI54" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ54" s="1">
         <f t="shared" si="0"/>
-        <v>2.2499754795633E+16</v>
+        <v>2.24997547949E+16</v>
       </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -6614,7 +6448,7 @@
         <v>338000000000</v>
       </c>
       <c r="O55" s="1">
-        <v>522000</v>
+        <v>0</v>
       </c>
       <c r="P55" s="1">
         <v>0</v>
@@ -6674,14 +6508,11 @@
         <v>0</v>
       </c>
       <c r="AI55" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ55" s="1">
         <f t="shared" si="0"/>
-        <v>1.9318150493472E+16</v>
+        <v>1.931815049295E+16</v>
       </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6725,7 +6556,7 @@
         <v>291000000000</v>
       </c>
       <c r="O56" s="1">
-        <v>334000</v>
+        <v>0</v>
       </c>
       <c r="P56" s="1">
         <v>0</v>
@@ -6785,14 +6616,11 @@
         <v>0</v>
       </c>
       <c r="AI56" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ56" s="1">
         <f t="shared" si="0"/>
-        <v>1.6616615191464E+16</v>
+        <v>1.661661519113E+16</v>
       </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6836,7 +6664,7 @@
         <v>250000000000</v>
       </c>
       <c r="O57" s="1">
-        <v>214000</v>
+        <v>0</v>
       </c>
       <c r="P57" s="1">
         <v>0</v>
@@ -6896,14 +6724,11 @@
         <v>0</v>
       </c>
       <c r="AI57" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ57" s="1">
         <f t="shared" si="0"/>
-        <v>1.4255497796014E+16</v>
+        <v>1.42554977958E+16</v>
       </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6947,7 +6772,7 @@
         <v>215000000000</v>
       </c>
       <c r="O58" s="1">
-        <v>169000</v>
+        <v>0</v>
       </c>
       <c r="P58" s="1">
         <v>0</v>
@@ -7007,14 +6832,11 @@
         <v>0</v>
       </c>
       <c r="AI58" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ58" s="1">
         <f t="shared" si="0"/>
-        <v>1.2304429994239E+16</v>
+        <v>1.230442999407E+16</v>
       </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -7058,7 +6880,7 @@
         <v>183000000000</v>
       </c>
       <c r="O59" s="1">
-        <v>117000</v>
+        <v>0</v>
       </c>
       <c r="P59" s="1">
         <v>0</v>
@@ -7118,14 +6940,11 @@
         <v>0</v>
       </c>
       <c r="AI59" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ59" s="1">
         <f t="shared" si="0"/>
-        <v>1.0583657799677E+16</v>
+        <v>1.058365779956E+16</v>
       </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -7169,7 +6988,7 @@
         <v>156000000000</v>
       </c>
       <c r="O60" s="1">
-        <v>69600</v>
+        <v>0</v>
       </c>
       <c r="P60" s="1">
         <v>0</v>
@@ -7229,14 +7048,11 @@
         <v>0</v>
       </c>
       <c r="AI60" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ60" s="1">
         <f t="shared" si="0"/>
-        <v>9103021704929600</v>
+        <v>9103021704860000</v>
       </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -7280,7 +7096,7 @@
         <v>132000000000</v>
       </c>
       <c r="O61" s="1">
-        <v>50800</v>
+        <v>0</v>
       </c>
       <c r="P61" s="1">
         <v>0</v>
@@ -7340,15 +7156,13 @@
         <v>0</v>
       </c>
       <c r="AI61" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ61" s="1">
         <f t="shared" si="0"/>
-        <v>7712271690540800</v>
+        <v>7712271690490000</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>